<commit_message>
Corrected fixed assets amounts in 'balance_sheet' file.
</commit_message>
<xml_diff>
--- a/Resources/balance_sheet.xlsx
+++ b/Resources/balance_sheet.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewSM/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewSM/FinTech/biz_acquisition_analysis/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC86F2C-F19E-1A4F-91A9-BF5D92B94206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D01B730-DC57-4E48-A865-8238CFDDE80D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="1560" windowWidth="27240" windowHeight="16440" xr2:uid="{DA96FBB8-E1C4-6C41-B7F0-11C3C5B3910B}"/>
+    <workbookView xWindow="11160" yWindow="1560" windowWidth="27240" windowHeight="16440" xr2:uid="{DA96FBB8-E1C4-6C41-B7F0-11C3C5B3910B}"/>
   </bookViews>
   <sheets>
     <sheet name="balance_sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,10 +466,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -505,7 +505,7 @@
         <v>20000</v>
       </c>
       <c r="F2" s="1">
-        <v>73000</v>
+        <v>60000</v>
       </c>
       <c r="G2" s="1">
         <v>15000</v>
@@ -541,7 +541,7 @@
         <v>20000</v>
       </c>
       <c r="F3" s="1">
-        <v>74000</v>
+        <v>61000</v>
       </c>
       <c r="G3" s="1">
         <v>15500</v>
@@ -578,7 +578,7 @@
         <v>20000</v>
       </c>
       <c r="F4" s="1">
-        <v>73000</v>
+        <v>60000</v>
       </c>
       <c r="G4" s="1">
         <v>15000</v>

</xml_diff>